<commit_message>
update the STBO results in ASR
</commit_message>
<xml_diff>
--- a/data/STBO_ASR_Experiment.xlsx
+++ b/data/STBO_ASR_Experiment.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cerence-my.sharepoint.com/personal/daijun_chen_cerence_com/Documents/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e403153b750a6671/项目/ASR_计算机实验设计/STBO/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DECCD9B0-7CBD-4875-B8A7-0069654DAC21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="29" documentId="8_{DECCD9B0-7CBD-4875-B8A7-0069654DAC21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F421BF12-49A4-41F4-8438-2A50A513652F}"/>
   <bookViews>
-    <workbookView xWindow="-16320" yWindow="-120" windowWidth="16440" windowHeight="28320" xr2:uid="{C6185F91-CF07-4BD3-913E-EC98F8C06A7F}"/>
+    <workbookView xWindow="-16320" yWindow="-120" windowWidth="16440" windowHeight="28320" activeTab="1" xr2:uid="{C6185F91-CF07-4BD3-913E-EC98F8C06A7F}"/>
   </bookViews>
   <sheets>
     <sheet name="MNC Experiment" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="12">
   <si>
     <t>response</t>
   </si>
@@ -69,13 +69,10 @@
     <t>knowledge</t>
   </si>
   <si>
-    <t>baseline</t>
-  </si>
-  <si>
     <t>cerencedrive_nav</t>
   </si>
   <si>
-    <t>response#factorybg#messaging#navprimary#knowledge</t>
+    <t>Baseline</t>
   </si>
 </sst>
 </file>
@@ -98,7 +95,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -123,6 +120,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -136,7 +145,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -144,6 +153,9 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -460,13 +472,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2651B82-C4E8-43A2-94B3-41FC6BA4515B}">
   <dimension ref="C6:H27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="10.5703125" customWidth="1"/>
+    <col min="5" max="6" width="12.140625" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" customWidth="1"/>
+    <col min="8" max="8" width="12.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="6" spans="3:8" x14ac:dyDescent="0.25">
@@ -475,11 +490,23 @@
       </c>
     </row>
     <row r="7" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C7" t="s">
+      <c r="C7" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D7" t="s">
-        <v>12</v>
+      <c r="D7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="H7" s="9" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="3:8" x14ac:dyDescent="0.25">
@@ -609,23 +636,23 @@
       </c>
     </row>
     <row r="14" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C14">
+      <c r="C14" s="8">
         <f t="shared" si="0"/>
         <v>16.800000000000004</v>
       </c>
       <c r="D14">
         <v>0.83199999999999996</v>
       </c>
-      <c r="E14">
+      <c r="E14" s="7">
         <v>4973</v>
       </c>
-      <c r="F14">
+      <c r="F14" s="7">
         <v>4624</v>
       </c>
-      <c r="G14">
+      <c r="G14" s="7">
         <v>355</v>
       </c>
-      <c r="H14">
+      <c r="H14" s="7">
         <v>1004</v>
       </c>
     </row>
@@ -909,19 +936,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3041E70C-F511-45CE-A922-6186A813816E}">
-  <dimension ref="E7:K34"/>
+  <dimension ref="E7:K33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C75" sqref="C75"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="3.5703125" customWidth="1"/>
     <col min="5" max="5" width="17.5703125" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" customWidth="1"/>
     <col min="8" max="8" width="11" customWidth="1"/>
     <col min="9" max="9" width="11.42578125" customWidth="1"/>
-    <col min="10" max="10" width="10.85546875" customWidth="1"/>
+    <col min="10" max="10" width="15.140625" customWidth="1"/>
     <col min="11" max="11" width="14.140625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -932,19 +960,19 @@
       <c r="F7" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G7" t="s">
+      <c r="G7" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="H7" t="s">
+      <c r="H7" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="I7" t="s">
+      <c r="I7" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="J7" t="s">
+      <c r="J7" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="K7" t="s">
+      <c r="K7" s="9" t="s">
         <v>9</v>
       </c>
     </row>
@@ -980,11 +1008,11 @@
     </row>
     <row r="10" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E10" s="4">
-        <f t="shared" ref="E10:E30" si="0">(8.6-F10)/8.6</f>
+        <f t="shared" ref="E10:E29" si="0">(8.6-F10)/8.6</f>
         <v>4.6511627906977202E-2</v>
       </c>
       <c r="F10">
-        <f t="shared" ref="F10:F30" si="1">(1-G10)*100</f>
+        <f t="shared" ref="F10:F29" si="1">(1-G10)*100</f>
         <v>8.1999999999999957</v>
       </c>
       <c r="G10">
@@ -1223,163 +1251,160 @@
     </row>
     <row r="24" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E24" s="4"/>
+      <c r="G24" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="25" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E25" s="4"/>
-      <c r="G25" t="s">
-        <v>3</v>
+      <c r="E25" s="4">
+        <f t="shared" si="0"/>
+        <v>0.23255813953488436</v>
+      </c>
+      <c r="F25">
+        <f t="shared" si="1"/>
+        <v>6.5999999999999943</v>
+      </c>
+      <c r="G25">
+        <v>0.93400000000000005</v>
+      </c>
+      <c r="H25">
+        <v>4973</v>
+      </c>
+      <c r="I25">
+        <v>4624</v>
+      </c>
+      <c r="J25">
+        <v>355</v>
+      </c>
+      <c r="K25">
+        <v>1004</v>
       </c>
     </row>
     <row r="26" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E26" s="4">
         <f t="shared" si="0"/>
-        <v>0.23255813953488436</v>
+        <v>4.6511627906977202E-2</v>
       </c>
       <c r="F26">
         <f t="shared" si="1"/>
-        <v>6.5999999999999943</v>
+        <v>8.1999999999999957</v>
       </c>
       <c r="G26">
-        <v>0.93400000000000005</v>
+        <v>0.91800000000000004</v>
       </c>
       <c r="H26">
-        <v>4973</v>
+        <v>3500</v>
       </c>
       <c r="I26">
-        <v>4624</v>
+        <v>1200</v>
       </c>
       <c r="J26">
-        <v>355</v>
+        <v>3000</v>
       </c>
       <c r="K26">
-        <v>1004</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="27" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E27" s="4">
         <f t="shared" si="0"/>
-        <v>4.6511627906977202E-2</v>
+        <v>0.16279069767441906</v>
       </c>
       <c r="F27">
         <f t="shared" si="1"/>
-        <v>8.1999999999999957</v>
+        <v>7.1999999999999957</v>
       </c>
       <c r="G27">
-        <v>0.91800000000000004</v>
+        <v>0.92800000000000005</v>
       </c>
       <c r="H27">
-        <v>3500</v>
+        <v>3607</v>
       </c>
       <c r="I27">
-        <v>1200</v>
+        <v>3135</v>
       </c>
       <c r="J27">
-        <v>3000</v>
+        <v>3158</v>
       </c>
       <c r="K27">
-        <v>1000</v>
+        <v>3369</v>
       </c>
     </row>
     <row r="28" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E28" s="4">
         <f t="shared" si="0"/>
-        <v>0.16279069767441906</v>
+        <v>-3.4883720930232232E-2</v>
       </c>
       <c r="F28">
         <f t="shared" si="1"/>
-        <v>7.1999999999999957</v>
+        <v>8.8999999999999968</v>
       </c>
       <c r="G28">
-        <v>0.92800000000000005</v>
+        <v>0.91100000000000003</v>
       </c>
       <c r="H28">
-        <v>3607</v>
+        <v>4131</v>
       </c>
       <c r="I28">
-        <v>3135</v>
+        <v>870</v>
       </c>
       <c r="J28">
-        <v>3158</v>
+        <v>1247</v>
       </c>
       <c r="K28">
-        <v>3369</v>
+        <v>3849</v>
       </c>
     </row>
     <row r="29" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E29" s="4">
         <f t="shared" si="0"/>
-        <v>-3.4883720930232232E-2</v>
+        <v>0.22093023255814009</v>
       </c>
       <c r="F29">
         <f t="shared" si="1"/>
-        <v>8.8999999999999968</v>
+        <v>6.6999999999999948</v>
       </c>
       <c r="G29">
-        <v>0.91100000000000003</v>
+        <v>0.93300000000000005</v>
       </c>
       <c r="H29">
-        <v>4131</v>
+        <v>3464</v>
       </c>
       <c r="I29">
-        <v>870</v>
+        <v>4126</v>
       </c>
       <c r="J29">
-        <v>1247</v>
+        <v>2185</v>
       </c>
       <c r="K29">
-        <v>3849</v>
-      </c>
-    </row>
-    <row r="30" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E30" s="4">
-        <f t="shared" si="0"/>
-        <v>0.22093023255814009</v>
-      </c>
-      <c r="F30">
-        <f t="shared" si="1"/>
-        <v>6.6999999999999948</v>
-      </c>
-      <c r="G30">
-        <v>0.93300000000000005</v>
-      </c>
-      <c r="H30">
-        <v>3464</v>
-      </c>
-      <c r="I30">
-        <v>4126</v>
-      </c>
-      <c r="J30">
-        <v>2185</v>
-      </c>
-      <c r="K30">
         <v>1528</v>
       </c>
     </row>
+    <row r="32" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="G32" t="s">
+        <v>11</v>
+      </c>
+    </row>
     <row r="33" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="G33" t="s">
+      <c r="E33" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="34" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E34" t="s">
-        <v>11</v>
-      </c>
-      <c r="F34" s="6">
+      <c r="F33" s="6">
         <v>8.6</v>
       </c>
-      <c r="G34" s="6">
+      <c r="G33" s="6">
         <v>0.91400000000000003</v>
       </c>
-      <c r="H34" s="6">
+      <c r="H33" s="6">
         <v>2519</v>
       </c>
-      <c r="I34" s="6">
+      <c r="I33" s="6">
         <v>931</v>
       </c>
-      <c r="J34" s="6">
+      <c r="J33" s="6">
         <v>3285</v>
       </c>
-      <c r="K34" s="6">
+      <c r="K33" s="6">
         <v>965</v>
       </c>
     </row>

</xml_diff>

<commit_message>
remove personal information before submit
</commit_message>
<xml_diff>
--- a/data/STBO_ASR_Experiment.xlsx
+++ b/data/STBO_ASR_Experiment.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e403153b750a6671/项目/ASR_计算机实验设计/STBO/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cerence-my.sharepoint.com/personal/daijun_chen_cerence_com/Documents/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="29" documentId="8_{DECCD9B0-7CBD-4875-B8A7-0069654DAC21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F421BF12-49A4-41F4-8438-2A50A513652F}"/>
+  <xr:revisionPtr revIDLastSave="41" documentId="8_{DECCD9B0-7CBD-4875-B8A7-0069654DAC21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E93FD491-837F-4368-8741-FCE62D58DE55}"/>
   <bookViews>
-    <workbookView xWindow="-16320" yWindow="-120" windowWidth="16440" windowHeight="28320" activeTab="1" xr2:uid="{C6185F91-CF07-4BD3-913E-EC98F8C06A7F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{C6185F91-CF07-4BD3-913E-EC98F8C06A7F}"/>
   </bookViews>
   <sheets>
     <sheet name="MNC Experiment" sheetId="2" r:id="rId1"/>
@@ -37,18 +37,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="11">
   <si>
     <t>response</t>
   </si>
   <si>
-    <t>GP</t>
-  </si>
-  <si>
     <t>STBO</t>
-  </si>
-  <si>
-    <t>BCBO</t>
   </si>
   <si>
     <t>WER</t>
@@ -57,22 +51,25 @@
     <t>WERR</t>
   </si>
   <si>
-    <t>factorybg</t>
+    <t>Baseline</t>
   </si>
   <si>
-    <t>messaging</t>
+    <t>LM2</t>
   </si>
   <si>
-    <t>navprimary</t>
+    <t>LM1</t>
   </si>
   <si>
-    <t>knowledge</t>
+    <t>LM3</t>
   </si>
   <si>
-    <t>cerencedrive_nav</t>
+    <t>LM4</t>
   </si>
   <si>
-    <t>Baseline</t>
+    <t>Diff-GP</t>
+  </si>
+  <si>
+    <t>EI</t>
   </si>
 </sst>
 </file>
@@ -473,7 +470,7 @@
   <dimension ref="C6:H27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M14" sqref="M14"/>
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -486,12 +483,12 @@
   <sheetData>
     <row r="6" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C7" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>0</v>
@@ -500,13 +497,13 @@
         <v>6</v>
       </c>
       <c r="F7" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="G7" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="G7" s="9" t="s">
+      <c r="H7" s="9" t="s">
         <v>8</v>
-      </c>
-      <c r="H7" s="9" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="8" spans="3:8" x14ac:dyDescent="0.25">
@@ -939,12 +936,12 @@
   <dimension ref="E7:K33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="3.5703125" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" customWidth="1"/>
     <col min="5" max="5" width="17.5703125" customWidth="1"/>
     <col min="7" max="7" width="13.28515625" customWidth="1"/>
     <col min="8" max="8" width="11" customWidth="1"/>
@@ -955,10 +952,10 @@
   <sheetData>
     <row r="7" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E7" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>0</v>
@@ -967,18 +964,18 @@
         <v>6</v>
       </c>
       <c r="I7" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="J7" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="J7" s="9" t="s">
+      <c r="K7" s="9" t="s">
         <v>8</v>
-      </c>
-      <c r="K7" s="9" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="8" spans="5:11" x14ac:dyDescent="0.25">
       <c r="G8" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="5:11" x14ac:dyDescent="0.25">
@@ -1115,7 +1112,7 @@
     <row r="16" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E16" s="4"/>
       <c r="G16" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="5:11" x14ac:dyDescent="0.25">
@@ -1252,7 +1249,7 @@
     <row r="24" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E24" s="4"/>
       <c r="G24" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
     </row>
     <row r="25" spans="5:11" x14ac:dyDescent="0.25">
@@ -1382,13 +1379,10 @@
     </row>
     <row r="32" spans="5:11" x14ac:dyDescent="0.25">
       <c r="G32" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="33" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E33" t="s">
-        <v>10</v>
-      </c>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="33" spans="6:11" x14ac:dyDescent="0.25">
       <c r="F33" s="6">
         <v>8.6</v>
       </c>

</xml_diff>